<commit_message>
filled in most other datapoints
</commit_message>
<xml_diff>
--- a/stats/Performance_paper_sheet.xlsx
+++ b/stats/Performance_paper_sheet.xlsx
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>ALL-10-FOLD-AVG</t>
   </si>
@@ -77,9 +78,6 @@
     <t>WASM Chrome</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>ASM.js Firefox</t>
   </si>
   <si>
@@ -93,6 +91,39 @@
   </si>
   <si>
     <t>Floyd-Warshall 1k</t>
+  </si>
+  <si>
+    <t>Firefox:</t>
+  </si>
+  <si>
+    <t>OS: Windows 10 Pro</t>
+  </si>
+  <si>
+    <t>Machine: Quad core i5-3550, 16GB DDR3 RAM, Sandisk Ultra II 480GB SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chrome: </t>
+  </si>
+  <si>
+    <t>Edge:</t>
+  </si>
+  <si>
+    <t>NodeJS:</t>
+  </si>
+  <si>
+    <t>v7.8.0</t>
+  </si>
+  <si>
+    <t>58.0.3029.110 (64-bit)</t>
+  </si>
+  <si>
+    <t>53.0.3 (32-bit)</t>
+  </si>
+  <si>
+    <t>40.15063.0.0</t>
+  </si>
+  <si>
+    <t>CONFIGURATION</t>
   </si>
 </sst>
 </file>
@@ -428,7 +459,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,9 +471,11 @@
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125"/>
     <col min="7" max="7" width="17.140625"/>
-    <col min="8" max="9" width="15.42578125"/>
+    <col min="8" max="8" width="15.42578125"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="18.85546875"/>
-    <col min="11" max="12" width="16.28515625"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -459,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -595,6 +628,9 @@
       <c r="D5">
         <v>10037</v>
       </c>
+      <c r="E5">
+        <v>1872</v>
+      </c>
       <c r="F5">
         <v>306</v>
       </c>
@@ -627,6 +663,9 @@
       <c r="D6">
         <v>2278</v>
       </c>
+      <c r="E6">
+        <v>1949</v>
+      </c>
       <c r="F6">
         <v>346</v>
       </c>
@@ -659,8 +698,11 @@
       <c r="D7">
         <v>520</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
+      <c r="E7">
+        <v>1934</v>
+      </c>
+      <c r="F7">
+        <v>366</v>
       </c>
       <c r="G7">
         <v>288</v>
@@ -680,7 +722,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>14.4</v>
@@ -691,6 +733,9 @@
       <c r="D8">
         <v>2954</v>
       </c>
+      <c r="E8">
+        <v>1613</v>
+      </c>
       <c r="F8">
         <v>389</v>
       </c>
@@ -712,7 +757,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>3.6</v>
@@ -723,8 +768,11 @@
       <c r="D9">
         <v>762</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
+      <c r="E9">
+        <v>1594</v>
+      </c>
+      <c r="F9">
+        <v>373</v>
       </c>
       <c r="G9">
         <v>306</v>
@@ -744,7 +792,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>29.6</v>
@@ -755,6 +803,9 @@
       <c r="D10">
         <v>5711</v>
       </c>
+      <c r="E10">
+        <v>1595</v>
+      </c>
       <c r="F10">
         <v>292</v>
       </c>
@@ -776,7 +827,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>13.1</v>
@@ -787,11 +838,14 @@
       <c r="D11">
         <v>1136</v>
       </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
+      <c r="E11">
+        <v>2303</v>
+      </c>
+      <c r="F11">
+        <v>471</v>
+      </c>
+      <c r="G11">
+        <v>533</v>
       </c>
       <c r="H11">
         <v>3780</v>
@@ -811,4 +865,66 @@
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed one effing data point
</commit_message>
<xml_diff>
--- a/stats/Performance_paper_sheet.xlsx
+++ b/stats/Performance_paper_sheet.xlsx
@@ -1,31 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\develop\wasm-experiments\stats\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView windowWidth="29173" windowHeight="16136" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
   <si>
     <t>ALL-10-FOLD-AVG</t>
   </si>
@@ -39,6 +29,9 @@
     <t>IntCompare 1e8</t>
   </si>
   <si>
+    <t>Floyd-Warshall 1k</t>
+  </si>
+  <si>
     <t>Permutations</t>
   </si>
   <si>
@@ -90,52 +83,54 @@
     <t>WASM Edge</t>
   </si>
   <si>
-    <t>Floyd-Warshall 1k</t>
+    <t>CONFIGURATION</t>
+  </si>
+  <si>
+    <t>Machine: Quad core i5-3550, 16GB DDR3 RAM, Sandisk Ultra II 480GB SSD</t>
+  </si>
+  <si>
+    <t>OS: Windows 10 Pro</t>
   </si>
   <si>
     <t>Firefox:</t>
   </si>
   <si>
-    <t>OS: Windows 10 Pro</t>
-  </si>
-  <si>
-    <t>Machine: Quad core i5-3550, 16GB DDR3 RAM, Sandisk Ultra II 480GB SSD</t>
+    <t>53.0.3 (32-bit)</t>
   </si>
   <si>
     <t xml:space="preserve">Chrome: </t>
   </si>
   <si>
+    <t>58.0.3029.110 (64-bit)</t>
+  </si>
+  <si>
     <t>Edge:</t>
   </si>
   <si>
+    <t>40.15063.0.0</t>
+  </si>
+  <si>
     <t>NodeJS:</t>
   </si>
   <si>
     <t>v7.8.0</t>
-  </si>
-  <si>
-    <t>58.0.3029.110 (64-bit)</t>
-  </si>
-  <si>
-    <t>53.0.3 (32-bit)</t>
-  </si>
-  <si>
-    <t>40.15063.0.0</t>
-  </si>
-  <si>
-    <t>CONFIGURATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -143,19 +138,355 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -163,10 +494,252 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
@@ -177,19 +750,58 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -198,7 +810,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="31363B"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -236,7 +848,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,7 +883,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,39 +1058,35 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="14.7109375"/>
-    <col min="2" max="2" width="12.85546875"/>
-    <col min="3" max="3" width="17.140625"/>
-    <col min="4" max="4" width="15.42578125"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125"/>
-    <col min="7" max="7" width="17.140625"/>
-    <col min="8" max="8" width="15.42578125"/>
+    <col min="1" max="1" width="14.7102803738318"/>
+    <col min="2" max="2" width="12.8598130841121"/>
+    <col min="3" max="3" width="17.1401869158878"/>
+    <col min="4" max="4" width="15.4299065420561"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="15.4299065420561"/>
+    <col min="7" max="7" width="17.1401869158878"/>
+    <col min="8" max="8" width="15.4299065420561"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875"/>
+    <col min="10" max="10" width="18.8598130841122"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625"/>
+    <col min="12" max="12" width="16.2897196261682"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,30 +1100,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>13.2</v>
@@ -526,6 +1134,9 @@
       <c r="D2">
         <v>1622</v>
       </c>
+      <c r="E2">
+        <v>687</v>
+      </c>
       <c r="F2">
         <v>153</v>
       </c>
@@ -545,9 +1156,9 @@
         <v>65227</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -580,9 +1191,9 @@
         <v>10087</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>22.6</v>
@@ -597,30 +1208,30 @@
         <v>2620</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>67.599999999999994</v>
+        <v>67.6</v>
       </c>
       <c r="C5">
         <v>1173</v>
@@ -650,9 +1261,9 @@
         <v>119323</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>12.2</v>
@@ -685,9 +1296,9 @@
         <v>120450</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -720,9 +1331,9 @@
         <v>112353</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>14.4</v>
@@ -755,9 +1366,9 @@
         <v>117550</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>3.6</v>
@@ -790,9 +1401,9 @@
         <v>108537</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>29.6</v>
@@ -825,9 +1436,9 @@
         <v>132141</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>13.1</v>
@@ -860,71 +1471,74 @@
         <v>148301</v>
       </c>
     </row>
-    <row r="20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="17.1" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins left="0.698611111111111" right="0.698611111111111" top="0.75" bottom="0.75" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.45" outlineLevelCol="2"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
produced new (final) plots
</commit_message>
<xml_diff>
--- a/stats/Performance_paper_sheet.xlsx
+++ b/stats/Performance_paper_sheet.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>RESULTS</t>
   </si>
@@ -150,7 +150,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,8 +181,14 @@
         <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -190,48 +196,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,7 +608,7 @@
   <dimension ref="B1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,387 +635,387 @@
       <c r="M1"/>
     </row>
     <row r="2" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="2">
         <v>13.2</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>371</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="2">
         <v>1622</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="3">
         <v>687</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="3">
         <v>153</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="2">
         <v>348</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="3">
         <v>1370</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="2">
         <v>619</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="4">
         <v>11068</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="2">
         <v>65227</v>
       </c>
     </row>
-    <row r="4" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>20</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="2">
         <v>804</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="2">
         <v>3891</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="2">
         <v>2495</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="2">
         <v>286</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="2">
         <v>311</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="2">
         <v>2488</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="2">
         <v>637</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="2">
         <v>4129</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="3">
         <v>10087</v>
       </c>
     </row>
-    <row r="5" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>22.6</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="2">
         <v>1375</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="2">
         <v>1392</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="4">
         <v>2620</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="5">
         <v>58831</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6">
+        <v>792</v>
+      </c>
+      <c r="I5" s="6">
+        <v>8682</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="11">
-        <v>8682</v>
-      </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="6" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>67.599999999999994</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <v>1173</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="4">
         <v>10037</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="2">
         <v>1872</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="2">
         <v>306</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="8">
         <v>615</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="2">
         <v>3275</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="4">
         <v>1143</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="2">
         <v>3249</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="2">
         <v>119323</v>
       </c>
     </row>
-    <row r="7" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>12.2</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="2">
         <v>806</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="2">
         <v>2278</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="2">
         <v>1949</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="2">
         <v>346</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="2">
         <v>346</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="2">
         <v>2082</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="2">
         <v>809</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="2">
         <v>2624</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="2">
         <v>120450</v>
       </c>
     </row>
-    <row r="8" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>2</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="2">
         <v>794</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="3">
         <v>520</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="2">
         <v>1934</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="2">
         <v>366</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="3">
         <v>288</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="2">
         <v>2033</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="2">
         <v>682</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="2">
         <v>2400</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="2">
         <v>112353</v>
       </c>
     </row>
-    <row r="9" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>14.4</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="2">
         <v>810</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="2">
         <v>2954</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="2">
         <v>1613</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="2">
         <v>389</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="2">
         <v>348</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="2">
         <v>2007</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="2">
         <v>708</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="2">
         <v>2406</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="2">
         <v>117550</v>
       </c>
     </row>
-    <row r="10" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <v>3.6</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="2">
         <v>830</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="2">
         <v>762</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="2">
         <v>1594</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="2">
         <v>373</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="2">
         <v>306</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="2">
         <v>1840</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="3">
         <v>610</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="3">
         <v>2074</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="2">
         <v>108537</v>
       </c>
     </row>
-    <row r="11" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <v>29.6</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="2">
         <v>1651</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="2">
         <v>5711</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="2">
         <v>1595</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="2">
         <v>292</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="2">
         <v>460</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="9">
         <v>2669</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="2">
         <v>987</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="2">
         <v>3267</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="2">
         <v>132141</v>
       </c>
     </row>
-    <row r="12" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <v>13.1</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="4">
         <v>1685</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="2">
         <v>1136</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="2">
         <v>2303</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="8">
         <v>471</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="2">
         <v>533</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="8">
         <v>3780</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="2">
         <v>1106</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="2">
         <v>3666</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="4">
         <v>148301</v>
       </c>
     </row>

</xml_diff>